<commit_message>
Edit and export Davide Gantt
</commit_message>
<xml_diff>
--- a/pp/gantt/DavideTasksAllocation.xlsx
+++ b/pp/gantt/DavideTasksAllocation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>Task #</t>
   </si>
@@ -132,6 +132,24 @@
   </si>
   <si>
     <t>Mario</t>
+  </si>
+  <si>
+    <t>Identification of use cases</t>
+  </si>
+  <si>
+    <t>Document revision</t>
+  </si>
+  <si>
+    <t>Integration test strategy</t>
+  </si>
+  <si>
+    <t>Definition of precedences</t>
+  </si>
+  <si>
+    <t>Integration test description</t>
+  </si>
+  <si>
+    <t>Data required</t>
   </si>
 </sst>
 </file>
@@ -494,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,14 +559,14 @@
         <v>6</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D27" si="0">CONCATENATE(NETWORKDAYS(E2,F2),"g")</f>
-        <v>20g</v>
+        <f t="shared" ref="D2:D34" si="0">CONCATENATE(NETWORKDAYS(E2,F2),"g")</f>
+        <v>46g</v>
       </c>
       <c r="E2" s="2">
-        <v>42688.333333333336</v>
+        <v>42660.333333333336</v>
       </c>
       <c r="F2" s="2">
-        <v>42715.666666666664</v>
+        <v>42723.666666666664</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -772,20 +790,20 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>1g</v>
       </c>
       <c r="E12" s="2">
-        <v>42676.333333333336</v>
+        <v>42671.333333333336</v>
       </c>
       <c r="F12" s="2">
-        <v>42676.666666666664</v>
+        <v>42671.666666666664</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -796,20 +814,20 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>7g</v>
+        <v>1g</v>
       </c>
       <c r="E13" s="2">
-        <v>42677.333333333336</v>
+        <v>42676.333333333336</v>
       </c>
       <c r="F13" s="2">
-        <v>42687.666666666664</v>
+        <v>42676.666666666664</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -820,7 +838,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
@@ -836,7 +854,7 @@
         <v>42687.666666666664</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -844,17 +862,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>2g</v>
+        <v>3g</v>
       </c>
       <c r="E15" s="2">
         <v>42677.333333333336</v>
       </c>
       <c r="F15" s="2">
-        <v>42678.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -865,79 +886,76 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>5g</v>
+        <v>2g</v>
       </c>
       <c r="E16" s="2">
-        <v>42679.333333333336</v>
+        <v>42677.333333333336</v>
       </c>
       <c r="F16" s="2">
-        <v>42685.666666666664</v>
+        <v>42678.666666666664</v>
       </c>
       <c r="G16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>3g</v>
       </c>
       <c r="E17" s="2">
-        <v>42688.333333333336</v>
+        <v>42677.333333333336</v>
       </c>
       <c r="F17" s="2">
-        <v>42690.666666666664</v>
+        <v>42681.666666666664</v>
       </c>
       <c r="G17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>4g</v>
       </c>
       <c r="E18" s="2">
-        <v>42688.333333333336</v>
+        <v>42682.333333333336</v>
       </c>
       <c r="F18" s="2">
-        <v>42690.666666666664</v>
+        <v>42685.666666666664</v>
       </c>
       <c r="G18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
@@ -953,15 +971,15 @@
         <v>42690.666666666664</v>
       </c>
       <c r="G19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -980,36 +998,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>2g</v>
+        <v>3g</v>
       </c>
       <c r="E21" s="2">
-        <v>42691.333333333336</v>
+        <v>42688.333333333336</v>
       </c>
       <c r="F21" s="2">
-        <v>42692.666666666664</v>
+        <v>42690.666666666664</v>
       </c>
       <c r="G21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
@@ -1019,128 +1037,300 @@
         <v>3g</v>
       </c>
       <c r="E22" s="2">
-        <v>42695.333333333336</v>
+        <v>42688.333333333336</v>
       </c>
       <c r="F22" s="2">
-        <v>42697.666666666664</v>
+        <v>42690.666666666664</v>
       </c>
       <c r="G22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
         <v>33</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>1g</v>
       </c>
       <c r="E23" s="2">
-        <v>42698.333333333336</v>
+        <v>42691.333333333336</v>
       </c>
       <c r="F23" s="2">
-        <v>42702.666666666664</v>
+        <v>42691.666666666664</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>2g</v>
       </c>
       <c r="E24" s="2">
-        <v>42703.333333333336</v>
+        <v>42692.333333333336</v>
       </c>
       <c r="F24" s="2">
-        <v>42705.666666666664</v>
+        <v>42695.666666666664</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>3g</v>
+        <v>2g</v>
       </c>
       <c r="E25" s="2">
-        <v>42706.333333333336</v>
+        <v>42696.333333333336</v>
       </c>
       <c r="F25" s="2">
-        <v>42710.666666666664</v>
+        <v>42697.666666666664</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>1g</v>
       </c>
       <c r="E26" s="2">
-        <v>42711.333333333336</v>
+        <v>42698.333333333336</v>
       </c>
       <c r="F26" s="2">
-        <v>42711.666666666664</v>
+        <v>42698.666666666664</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>4g</v>
+      </c>
+      <c r="E27" s="2">
+        <v>42699.333333333336</v>
+      </c>
+      <c r="F27" s="2">
+        <v>42704.666666666664</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E28" s="2">
+        <v>42705.333333333336</v>
+      </c>
+      <c r="F28" s="2">
+        <v>42705.666666666664</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="C27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" t="str">
+      <c r="C29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" t="str">
         <f t="shared" si="0"/>
         <v>1g</v>
       </c>
-      <c r="E27" s="2">
-        <v>42713.333333333336</v>
-      </c>
-      <c r="F27" s="2">
-        <v>42713.666666666664</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
+      <c r="E29" s="2">
+        <v>42706.333333333336</v>
+      </c>
+      <c r="F29" s="2">
+        <v>42706.666666666664</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E30" s="2">
+        <v>42716.333333333336</v>
+      </c>
+      <c r="F30" s="2">
+        <v>42716.666666666664</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E31" s="2">
+        <v>42716.333333333336</v>
+      </c>
+      <c r="F31" s="2">
+        <v>42716.666666666664</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>3g</v>
+      </c>
+      <c r="E32" s="2">
+        <v>42717.333333333336</v>
+      </c>
+      <c r="F32" s="2">
+        <v>42719.666666666664</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>1g</v>
+      </c>
+      <c r="E33" s="2">
+        <v>42720.333333333336</v>
+      </c>
+      <c r="F33" s="2">
+        <v>42720.666666666664</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>2g</v>
+      </c>
+      <c r="E34" s="2">
+        <v>42720.333333333336</v>
+      </c>
+      <c r="F34" s="2">
+        <v>42723.666666666664</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>